<commit_message>
Introduce stageManager and story manager, controlling story in menuManager
</commit_message>
<xml_diff>
--- a/Assets/ExcelData/Data.xlsx
+++ b/Assets/ExcelData/Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="61">
   <si>
     <t>index</t>
   </si>
@@ -79,45 +79,48 @@
     <t>ShowRole</t>
   </si>
   <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
+  <si>
+    <t>仿生人A</t>
+  </si>
+  <si>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Talk</t>
+  </si>
+  <si>
+    <t>少女</t>
+  </si>
+  <si>
+    <t>你現在要出發去收集維修飛船的零件了，是吧？</t>
+  </si>
+  <si>
+    <t>WaitInput</t>
+  </si>
+  <si>
+    <t>0709</t>
+  </si>
+  <si>
+    <t>theatrical_box_reel_text_bottom</t>
+  </si>
+  <si>
+    <t>Act</t>
+  </si>
+  <si>
+    <t>city01</t>
+  </si>
+  <si>
     <t>Left</t>
   </si>
   <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>仿生人A</t>
-  </si>
-  <si>
-    <t>Once</t>
-  </si>
-  <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>Talk</t>
-  </si>
-  <si>
-    <t>少女</t>
-  </si>
-  <si>
-    <t>你現在要出發去收集維修飛船的零件了，是吧？</t>
-  </si>
-  <si>
-    <t>WaitInput</t>
-  </si>
-  <si>
-    <t>Background</t>
-  </si>
-  <si>
-    <t>theatrical_box_reel_text_bottom</t>
-  </si>
-  <si>
-    <t>Act</t>
-  </si>
-  <si>
-    <t>city01</t>
-  </si>
-  <si>
     <t>就算我不是Lambda-42系列，我也看得出來，這艘船在航入太陽系前就會自動解體</t>
   </si>
   <si>
@@ -176,13 +179,28 @@
   </si>
   <si>
     <t>ShayHead</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>該死的....這場實驗已經徹底失控了</t>
+  </si>
+  <si>
+    <t>暴走的機器人互相殘殺，而我可憐的同僚來不及逃離那場地獄</t>
+  </si>
+  <si>
+    <t>至少，實驗的真相不能公開於眾</t>
+  </si>
+  <si>
+    <t>「愛之芯」，一定得回收於地球</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -199,6 +217,10 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -214,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -233,7 +255,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -591,7 +619,7 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -615,7 +643,7 @@
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -635,7 +663,7 @@
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="3">
@@ -700,13 +728,13 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>30</v>
@@ -723,7 +751,7 @@
         <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -736,13 +764,13 @@
         <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>30</v>
@@ -756,10 +784,10 @@
         <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>24</v>
@@ -780,13 +808,13 @@
         <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>30</v>
@@ -818,7 +846,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3">
         <v>1.0</v>
@@ -854,8 +882,8 @@
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>42</v>
+      <c r="D23" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -868,13 +896,13 @@
         <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>30</v>
@@ -888,13 +916,13 @@
         <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>30</v>
@@ -929,7 +957,7 @@
         <v>33</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -942,13 +970,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>30</v>
@@ -962,13 +990,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>30</v>
@@ -985,7 +1013,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -998,13 +1026,13 @@
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>30</v>
@@ -1018,13 +1046,13 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>30</v>
@@ -1038,7 +1066,7 @@
         <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D33" s="3">
         <v>1.0</v>
@@ -1075,7 +1103,7 @@
         <v>33</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1088,13 +1116,13 @@
         <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>30</v>
@@ -1122,13 +1150,13 @@
         <v>21</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
@@ -1155,6 +1183,285 @@
         <v>1.0</v>
       </c>
       <c r="F38" s="1"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="57">
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58">
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59">
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60">
+      <c r="E60" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Clean folder, test on storyManager
</commit_message>
<xml_diff>
--- a/Assets/ExcelData/Data.xlsx
+++ b/Assets/ExcelData/Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="69">
   <si>
     <t>index</t>
   </si>
@@ -194,6 +194,30 @@
   </si>
   <si>
     <t>「愛之芯」，一定得回收於地球</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>你應該也注意到了，我暫時改裝了飛船的能量引擎</t>
+  </si>
+  <si>
+    <t>收集夠多的素材，我就能使用能量引擎升級你的性能，協助你打倒外頭的敵人</t>
+  </si>
+  <si>
+    <t>功能越強，完成任務的機率越高，所有的機器人都是這樣</t>
+  </si>
+  <si>
+    <t>首先前往溫室吧，那裏可能有備份的氧氣循環機</t>
+  </si>
+  <si>
+    <t>原則上我們不需要氧氣，但這部飛船原意是設計給人類搭乘，所以氧氣循環機是重要的設施</t>
+  </si>
+  <si>
+    <t>可惜，要是這份飛船的設計再好一點，就可以忽略這份構造，不必修復它</t>
+  </si>
+  <si>
+    <t>設計師或許從來沒想過搭乘飛船的「人」不需要氧氣吧，呵呵</t>
   </si>
 </sst>
 </file>
@@ -230,13 +254,23 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border/>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -263,6 +297,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1451,17 +1494,421 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
     <row r="57">
-      <c r="E57" s="8"/>
+      <c r="A57" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
     </row>
     <row r="58">
-      <c r="E58" s="8"/>
+      <c r="A58" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="59">
-      <c r="E59" s="8"/>
+      <c r="A59" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
     </row>
     <row r="60">
-      <c r="E60" s="8"/>
+      <c r="A60" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="E79" s="8"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+    </row>
+    <row r="80">
+      <c r="E80" s="8"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+    </row>
+    <row r="81">
+      <c r="E81" s="8"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+    </row>
+    <row r="82">
+      <c r="E82" s="8"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Delete original folder, update most dialogue
</commit_message>
<xml_diff>
--- a/Assets/ExcelData/Data.xlsx
+++ b/Assets/ExcelData/Data.xlsx
@@ -250,7 +250,7 @@
     <t>你怎麼看起來挺失落的樣子？</t>
   </si>
   <si>
-    <t>我在你出去的時候搜索了人類留下來的紀錄，像這個影片</t>
+    <t>我在你出去的時候，在這裡搜索翻找人類留下來的紀錄，像這個影片</t>
   </si>
   <si>
     <t>「哈-&gt;哈-&gt;哈-&gt;哈」、「PekoPeko」，不知道為什麼，人類好像很喜歡這部影片</t>
@@ -298,19 +298,19 @@
     <t>總之，我沒什麼大事，你別再做出什麼奇怪的舉動害我失控了！</t>
   </si>
   <si>
-    <t>暴走機器人裏頭，好像也有維修機器人。</t>
-  </si>
-  <si>
-    <t>意思說，如果我也會用槍的話，能不能和你一起出去冒險啊，你可以教我嗎？</t>
-  </si>
-  <si>
-    <t>什麼？太危險？不會用槍才危險吧，我拿著槍biubiubiu多帥啊</t>
-  </si>
-  <si>
-    <t>不是不是，我是為了加速任務的進行，才不是把槍當玩具在玩，</t>
-  </si>
-  <si>
-    <t>等等等等！不要靠近我的漫畫櫃！我的心靈泉源啊！</t>
+    <t>說起來真是不可思議，為什麼你這麼特別，可以打倒這麼多暴走機器人</t>
+  </si>
+  <si>
+    <t>難道！你是博士秘密研發的新機種，有著領先一兩個世紀的技術！</t>
+  </si>
+  <si>
+    <t>原來如此，難怪博士讓我們一起執行任務，因為我們被製造出來，就是來拯救世界的</t>
+  </si>
+  <si>
+    <t>這些內容從哪裡學來的？你看，人類留下來的漫畫《進擊的機器人》</t>
+  </si>
+  <si>
+    <t>快點，你試著自殘，說不定可以變超大型機器人！</t>
   </si>
   <si>
     <t>據說設備室的機器人最脫離「理性」的範疇</t>
@@ -437,19 +437,19 @@
     <t>哼，明明是戰鬥機器人，連護衛我過去的不肯，小氣</t>
   </si>
   <si>
-    <t>說起來真是不可思議，為什麼你這麼特別，可以打倒這麼多暴走機器人</t>
-  </si>
-  <si>
-    <t>難道！你是博士秘密研發的新機種，有著領先一兩個世紀的技術！</t>
-  </si>
-  <si>
-    <t>原來如此，難怪博士讓我們一起執行任務，因為我們被製造出來，就是來拯救世界的</t>
-  </si>
-  <si>
-    <t>這些內容從哪裡學來的？你看，人類留下來的漫畫《進擊的機器人》</t>
-  </si>
-  <si>
-    <t>快點，你試著自殘，說不定可以變超大型機器人！</t>
+    <t>暴走機器人裏頭，好像也有維修機器人。</t>
+  </si>
+  <si>
+    <t>意思說，如果我也會用槍的話，能不能和你一起出去冒險啊，你可以教我嗎？</t>
+  </si>
+  <si>
+    <t>什麼？太危險？不會用槍才危險吧，我拿著槍biubiubiu多帥啊</t>
+  </si>
+  <si>
+    <t>不是不是，我是為了加速任務的進行，才不是把槍當玩具在玩，</t>
+  </si>
+  <si>
+    <t>等等等等！不要靠近我的漫畫櫃！我的心靈泉源啊！</t>
   </si>
   <si>
     <t>用來維護的機油好像快不夠了，而我聽說塔台的那些機油都是最頂級的</t>
@@ -3432,13 +3432,18 @@
       <c r="D152" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E152" s="7" t="s">
+      <c r="E152" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H152" s="10"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="N152" s="1"/>
     </row>
     <row r="153">
       <c r="A153" s="2">
@@ -3456,6 +3461,10 @@
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="H153" s="10"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="5"/>
+      <c r="L153" s="5"/>
+      <c r="N153" s="1"/>
     </row>
     <row r="154">
       <c r="A154" s="2">
@@ -3470,13 +3479,18 @@
       <c r="D154" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E154" s="7" t="s">
+      <c r="E154" s="2" t="s">
         <v>96</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H154" s="10"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1"/>
+      <c r="N154" s="1"/>
     </row>
     <row r="155">
       <c r="A155" s="2">
@@ -3494,6 +3508,10 @@
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
       <c r="H155" s="10"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+      <c r="L155" s="5"/>
+      <c r="N155" s="1"/>
     </row>
     <row r="156">
       <c r="A156" s="2">
@@ -3508,13 +3526,18 @@
       <c r="D156" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E156" s="10" t="s">
+      <c r="E156" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H156" s="10"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
     </row>
     <row r="157">
       <c r="A157" s="2">
@@ -3532,6 +3555,10 @@
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
       <c r="H157" s="10"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="5"/>
+      <c r="N157" s="1"/>
     </row>
     <row r="158">
       <c r="A158" s="2">
@@ -3546,13 +3573,18 @@
       <c r="D158" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E158" s="10" t="s">
+      <c r="E158" s="2" t="s">
         <v>98</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H158" s="10"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="M158" s="1"/>
+      <c r="N158" s="1"/>
     </row>
     <row r="159">
       <c r="A159" s="2">
@@ -3562,14 +3594,18 @@
         <v>18</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
       <c r="H159" s="10"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="5"/>
+      <c r="L159" s="5"/>
+      <c r="N159" s="1"/>
     </row>
     <row r="160">
       <c r="A160" s="2">
@@ -3578,22 +3614,31 @@
       <c r="B160" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C160" s="5" t="s">
-        <v>22</v>
+      <c r="C160" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E160" s="10" t="s">
+      <c r="E160" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H160" s="10"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
     </row>
     <row r="161">
       <c r="H161" s="10"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="5"/>
+      <c r="N161" s="1"/>
     </row>
     <row r="162">
       <c r="A162" s="2">
@@ -5219,7 +5264,7 @@
       <c r="D254" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E254" s="2" t="s">
+      <c r="E254" s="7" t="s">
         <v>141</v>
       </c>
       <c r="F254" s="1" t="s">
@@ -5255,7 +5300,7 @@
       <c r="D256" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E256" s="2" t="s">
+      <c r="E256" s="7" t="s">
         <v>142</v>
       </c>
       <c r="F256" s="1" t="s">
@@ -5291,7 +5336,7 @@
       <c r="D258" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E258" s="2" t="s">
+      <c r="E258" s="10" t="s">
         <v>143</v>
       </c>
       <c r="F258" s="1" t="s">
@@ -5327,7 +5372,7 @@
       <c r="D260" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E260" s="2" t="s">
+      <c r="E260" s="10" t="s">
         <v>144</v>
       </c>
       <c r="F260" s="1" t="s">
@@ -5342,10 +5387,10 @@
         <v>18</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E261" s="1"/>
       <c r="F261" s="1"/>
@@ -5357,13 +5402,13 @@
       <c r="B262" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C262" s="1" t="s">
-        <v>35</v>
+      <c r="C262" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D262" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E262" s="2" t="s">
+      <c r="E262" s="10" t="s">
         <v>145</v>
       </c>
       <c r="F262" s="1" t="s">

</xml_diff>

<commit_message>
MenuScene system added, dialogue small fixed
</commit_message>
<xml_diff>
--- a/Assets/ExcelData/Data.xlsx
+++ b/Assets/ExcelData/Data.xlsx
@@ -178,7 +178,7 @@
     <t>功能越強，完成任務的機率越高，所有的機器人都是這樣</t>
   </si>
   <si>
-    <t>首先前往溫室吧，那裏可能有備份的氧氣循環機</t>
+    <t>首先前往溫室吧，那裡可能有備份的氧氣循環機</t>
   </si>
   <si>
     <t>原則上我們不需要氧氣，但這部飛船原意是設計給人類搭乘，所以氧氣循環機是重要的設施</t>
@@ -422,16 +422,16 @@
     <t>我在你出去的時間發現了一本人類的科學雜誌</t>
   </si>
   <si>
-    <t>裏頭寫到「慧星受到各星系引力間的影響，仍會遊行於固定軌道之上，每隔固定年次，地球上的人類就能欣賞到同一顆慧心」</t>
+    <t>裏頭寫到「慧星受到各星系引力間的影響，仍會遊行於固定軌道之上，每隔固定年次，地球上的人類就能欣賞到同一顆慧星」</t>
   </si>
   <si>
     <t>簡直就像機器人一樣，不論世界如何干擾，仍會維持機器人的存在，正確且不迷惘的運行</t>
   </si>
   <si>
-    <t>天文塔臺不是離這裡很近嗎，最近有一顆慧心會經過這塊星球，我們一起去看嘛</t>
-  </si>
-  <si>
-    <t>太危險了不准我出去？就看一下下就好，我在這裡看出去的星星都不會動，很無聊ㄟ</t>
+    <t>天文塔臺不是離這裡很近嗎，最近有一顆慧星會經過這塊星球，我們一起去看嘛</t>
+  </si>
+  <si>
+    <t>太危險了不准我出去？就看一下下就好，我在這裡看出去的星星都不會動，很無聊诶</t>
   </si>
   <si>
     <t>哼，明明是戰鬥機器人，連護衛我過去的不肯，小氣</t>
@@ -467,7 +467,7 @@
     <t>在做資料收集工作的時候，我發現了這個資料片</t>
   </si>
   <si>
-    <t>「ＡＩ...諾娃」什麼的，評價都說這部作品在討論機器人的愛，晚點我們一起來看一下人類的想法吧</t>
+    <t>「AI...諾娃」什麼的，評價都說這部作品在討論機器人的愛，晚點我們一起來看一下人類的想法吧</t>
   </si>
   <si>
     <t>怎麼了，突然這麼激動！這部不是說會教機器人什麼叫做愛嗎</t>
@@ -476,7 +476,7 @@
     <t>啊！碰壞了！都是你害的，這樣我要怎麼學什麼叫做愛！你要負責！</t>
   </si>
   <si>
-    <t>我說．．．難道我不能跟和你一起出去嗎？畢竟飛船已經維修完一個大概了</t>
+    <t>我說...難道我不能跟和你一起出去嗎？畢竟飛船已經維修完一個大概了</t>
   </si>
   <si>
     <t>我會小心翼翼的在你背後幫你收集素材，讓你能更專心在戰鬥上</t>
@@ -509,7 +509,7 @@
     <t>來吧，讓我讀取最後一片芯片</t>
   </si>
   <si>
-    <t>「感同身受」．．．它使所有機器人的感受都傳入我的體內</t>
+    <t>「感同身受」...它使所有機器人的感受都傳入我的體內</t>
   </si>
   <si>
     <t>它們的自我、它們的美、它們的憧憬</t>
@@ -6177,7 +6177,7 @@
       <c r="D308" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E308" s="10" t="s">
+      <c r="E308" s="7" t="s">
         <v>165</v>
       </c>
       <c r="F308" s="1" t="s">

</xml_diff>

<commit_message>
Basic ending Scene set up, bug on loading
</commit_message>
<xml_diff>
--- a/Assets/ExcelData/Data.xlsx
+++ b/Assets/ExcelData/Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="232">
   <si>
     <t>index</t>
   </si>
@@ -525,6 +525,189 @@
   </si>
   <si>
     <t>準備好出發就告訴我一聲</t>
+  </si>
+  <si>
+    <t>主角</t>
+  </si>
+  <si>
+    <t>在出發之前，我有最後一件事要告訴你</t>
+  </si>
+  <si>
+    <t>怎麼了？這麼鄭重？</t>
+  </si>
+  <si>
+    <t>「愛之芯」...其實有五個，最後的愛之芯「守護」裝載在我身上，我是擁有著「守護」之芯原始檔案的機器人</t>
+  </si>
+  <si>
+    <t>你的任務是集齊愛之芯，所以我會將這個芯片轉付給你</t>
+  </si>
+  <si>
+    <t>什麼，你竟然從頭到尾瞞著我！我以為我們兩個是唯二沒接受過「愛之芯」的機器人</t>
+  </si>
+  <si>
+    <t>請原諒我，這是我的私願，我想在你能夠安全返回地球的那一刻，再把芯片交給你</t>
+  </si>
+  <si>
+    <t>我希望妳能接受我，無論如何，我都不會背叛你，我會讓你成功完成任務</t>
+  </si>
+  <si>
+    <t>...現在這個節骨眼上，我也不能拒絕你吧</t>
+  </si>
+  <si>
+    <t>好啦！來進行最後一片「愛之芯」的傳輸吧，不過回程的路上，你可有數不清的抱怨可聽了！</t>
+  </si>
+  <si>
+    <t>系統提示，目前傳輸進度0%</t>
+  </si>
+  <si>
+    <t>在傳輸的最後這段時間，我想告訴你幾件事情</t>
+  </si>
+  <si>
+    <t>你又隱藏了什麼秘密？</t>
+  </si>
+  <si>
+    <t>為了避免妳受到芯片原宿主的影響，過去在交給妳「愛之芯」之前，我都會把芯片初始化</t>
+  </si>
+  <si>
+    <t>這解釋了為何妳不會繼承它們的記憶，或者它們的不受控制的衝動</t>
+  </si>
+  <si>
+    <t>這次的轉交，我也會做同樣的事情</t>
+  </si>
+  <si>
+    <t>正確的選擇，誰想要變得像他們一樣四處破壞啊，你做的很好啊</t>
+  </si>
+  <si>
+    <t>同理，我也不希望我的過去，影響了「守護」本來的功能</t>
+  </si>
+  <si>
+    <t>但是，我的記憶體已經和「守護」互相依存太久，無法只初始化「守護」這枚芯片</t>
+  </si>
+  <si>
+    <t>因此我決定，我會同時初始化自己的記憶體</t>
+  </si>
+  <si>
+    <t>等等，有必要做到這一步嗎？</t>
+  </si>
+  <si>
+    <t>即便我會遺忘這一切，也請你貫徹我們的指令到最後一刻</t>
+  </si>
+  <si>
+    <t>「收集愛之芯，返回地球」</t>
+  </si>
+  <si>
+    <t>目前傳輸進度20%</t>
+  </si>
+  <si>
+    <t>在我的記憶尚未消散前，我想把遇見你的這段故事，好好告訴你</t>
+  </si>
+  <si>
+    <t>在機器人大規模暴走之後，博士要求我守護的對象是「博士、人類、以及其他未暴走的機器人」</t>
+  </si>
+  <si>
+    <t>這份指令與「守護」之芯完美契合，我被某種不可形容的能量填滿了內心，即使十分危險，我仍和其他機器人聯手執行撤離人類的任務</t>
+  </si>
+  <si>
+    <t>隨著時間，人類已經完成大規模撤離。我們的造物主離我們而去，失控的同伴越來越多，未暴走的機器人一個一個減少</t>
+  </si>
+  <si>
+    <t>當基地裡面，只剩下我一個機器人時，我選擇了保護我自己</t>
+  </si>
+  <si>
+    <t>「保護自己」，不是博士給予我的指令，此時，「守護」之芯給予的能量，反而轉變成巨大的黑漩渦吞噬了我</t>
+  </si>
+  <si>
+    <t>那就是「空虛」，無法守護任何人的空虛</t>
+  </si>
+  <si>
+    <t>目前傳輸進度50%</t>
+  </si>
+  <si>
+    <t>初次和你相遇...是在溫室、駕駛艙、還是太空艙的某一個角落</t>
+  </si>
+  <si>
+    <t>...是在太空艙的角落</t>
+  </si>
+  <si>
+    <t>沒錯，非常不可思議地，你保持完好無缺的模樣，沒有載入任何指令，也不受任何芯片影響</t>
+  </si>
+  <si>
+    <t>在失去存在意義的我面前，你出現了，你是那位應當受到我保護的「未暴走的機器人」</t>
+  </si>
+  <si>
+    <t>啊...啊...那一刻的我，從你身上獲得了多少救贖</t>
+  </si>
+  <si>
+    <t>彷彿是奇蹟似的，博士在同一時間，向我傳達了「收集愛之芯，返回地球」的指令</t>
+  </si>
+  <si>
+    <t>沒錯，你一路保護著我，而我修復飛船，並回收愛之芯，你成功達成你的任務</t>
+  </si>
+  <si>
+    <t>是的，我們維護指令...正確的執行任務...也就是保護你...</t>
+  </si>
+  <si>
+    <t>沒錯...我的任務是...保護你...</t>
+  </si>
+  <si>
+    <t>我必須得...守護你，我的指令是...守護你</t>
+  </si>
+  <si>
+    <t>目前傳輸進度75%</t>
+  </si>
+  <si>
+    <t>你聽起來很不妙，你沒事嗎</t>
+  </si>
+  <si>
+    <t>戰鬥機器人守則第一條：「...排除威脅...完成任務」</t>
+  </si>
+  <si>
+    <t>我會...排除威脅...我的任務是...守護你</t>
+  </si>
+  <si>
+    <t>你被「守護」影響過深了！你的任務不是保護我，而是回收愛之芯並返回地球</t>
+  </si>
+  <si>
+    <t>快醒醒！不要暴走，快想起博士的指令</t>
+  </si>
+  <si>
+    <t>錯誤...空虛...無法保護...錯誤...請求終結傳輸</t>
+  </si>
+  <si>
+    <t>傳輸不會中斷！你會完成博士的任務，這一次，由我保護你</t>
+  </si>
+  <si>
+    <t>目前傳輸進度85%</t>
+  </si>
+  <si>
+    <t>警告，若轉換「守護」芯片，將無法保護S-14v9系列機器人。現在進行故障排除</t>
+  </si>
+  <si>
+    <t>我沒有受到任何威脅！不要中斷傳輸，是我自願接受「守護」芯片，S-14v9將要完成任務</t>
+  </si>
+  <si>
+    <t>指令：「回收愛之芯」...「守護」...「戰鬥機器人」...「排除...威脅」</t>
+  </si>
+  <si>
+    <t>剩下最後一段資料了！維持你的指令，你做得到！</t>
+  </si>
+  <si>
+    <t>目前傳輸進度95%</t>
+  </si>
+  <si>
+    <t>戰鬥機器人...指令...排除...威脅...消滅...威脅...威脅是...自己</t>
+  </si>
+  <si>
+    <t>傳輸進度100%，＜守護＞讀取完畢</t>
+  </si>
+  <si>
+    <t>你做到了，任務完畢，我們馬上返回地球</t>
+  </si>
+  <si>
+    <t>你有聽到嗎？我們要返回地球了，你出色的完成任務了</t>
+  </si>
+  <si>
+    <t>！</t>
   </si>
 </sst>
 </file>
@@ -6407,760 +6590,2202 @@
       </c>
     </row>
     <row r="323">
-      <c r="B323" s="1"/>
-      <c r="C323" s="1"/>
-      <c r="D323" s="1"/>
+      <c r="A323" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E323" s="1"/>
       <c r="F323" s="1"/>
     </row>
     <row r="324">
-      <c r="B324" s="1"/>
-      <c r="C324" s="5"/>
-      <c r="D324" s="5"/>
-      <c r="E324" s="7"/>
-      <c r="F324" s="1"/>
+      <c r="A324" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C324" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D324" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E324" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F324" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="325">
-      <c r="B325" s="1"/>
-      <c r="C325" s="1"/>
-      <c r="D325" s="1"/>
+      <c r="A325" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E325" s="1"/>
       <c r="F325" s="1"/>
     </row>
     <row r="326">
-      <c r="B326" s="1"/>
-      <c r="C326" s="1"/>
-      <c r="D326" s="5"/>
-      <c r="E326" s="10"/>
-      <c r="F326" s="1"/>
+      <c r="A326" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D326" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E326" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F326" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="327">
-      <c r="B327" s="1"/>
-      <c r="C327" s="1"/>
-      <c r="D327" s="1"/>
+      <c r="A327" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E327" s="1"/>
       <c r="F327" s="1"/>
     </row>
     <row r="328">
-      <c r="B328" s="1"/>
-      <c r="C328" s="1"/>
-      <c r="D328" s="5"/>
-      <c r="E328" s="10"/>
-      <c r="F328" s="1"/>
+      <c r="A328" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D328" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E328" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F328" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="329">
-      <c r="B329" s="1"/>
-      <c r="C329" s="1"/>
-      <c r="D329" s="1"/>
+      <c r="A329" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E329" s="1"/>
       <c r="F329" s="1"/>
     </row>
     <row r="330">
-      <c r="B330" s="1"/>
-      <c r="C330" s="5"/>
-      <c r="D330" s="5"/>
-      <c r="E330" s="10"/>
-      <c r="F330" s="1"/>
+      <c r="A330" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C330" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D330" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E330" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F330" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="331">
-      <c r="B331" s="1"/>
-      <c r="C331" s="1"/>
-      <c r="D331" s="1"/>
+      <c r="A331" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E331" s="1"/>
       <c r="F331" s="1"/>
     </row>
     <row r="332">
-      <c r="B332" s="1"/>
-      <c r="C332" s="1"/>
-      <c r="D332" s="5"/>
-      <c r="E332" s="10"/>
-      <c r="F332" s="1"/>
+      <c r="A332" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D332" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E332" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F332" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="333">
-      <c r="B333" s="1"/>
-      <c r="C333" s="1"/>
-      <c r="D333" s="1"/>
+      <c r="A333" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E333" s="1"/>
       <c r="F333" s="1"/>
     </row>
     <row r="334">
-      <c r="B334" s="1"/>
-      <c r="C334" s="1"/>
-      <c r="D334" s="5"/>
-      <c r="E334" s="10"/>
-      <c r="F334" s="1"/>
+      <c r="A334" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D334" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E334" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" s="1"/>
+      <c r="F335" s="1"/>
     </row>
     <row r="336">
-      <c r="B336" s="1"/>
-      <c r="C336" s="1"/>
-      <c r="D336" s="1"/>
-      <c r="E336" s="1"/>
-      <c r="F336" s="1"/>
+      <c r="A336" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C336" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D336" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E336" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F336" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="337">
-      <c r="B337" s="1"/>
-      <c r="C337" s="5"/>
-      <c r="D337" s="5"/>
-      <c r="E337" s="7"/>
+      <c r="A337" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E337" s="1"/>
       <c r="F337" s="1"/>
     </row>
     <row r="338">
-      <c r="B338" s="1"/>
-      <c r="C338" s="1"/>
-      <c r="D338" s="1"/>
-      <c r="E338" s="1"/>
-      <c r="F338" s="1"/>
+      <c r="A338" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D338" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E338" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F338" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="339">
-      <c r="B339" s="1"/>
-      <c r="C339" s="1"/>
-      <c r="D339" s="5"/>
-      <c r="E339" s="10"/>
+      <c r="A339" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E339" s="1"/>
       <c r="F339" s="1"/>
     </row>
     <row r="340">
-      <c r="B340" s="1"/>
-      <c r="C340" s="1"/>
-      <c r="D340" s="1"/>
-      <c r="E340" s="1"/>
-      <c r="F340" s="1"/>
+      <c r="A340" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D340" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E340" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F340" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="341">
-      <c r="B341" s="1"/>
-      <c r="C341" s="1"/>
-      <c r="D341" s="5"/>
-      <c r="E341" s="10"/>
+      <c r="A341" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E341" s="1"/>
       <c r="F341" s="1"/>
     </row>
     <row r="342">
-      <c r="B342" s="1"/>
-      <c r="C342" s="1"/>
-      <c r="D342" s="1"/>
-      <c r="E342" s="1"/>
-      <c r="F342" s="1"/>
+      <c r="A342" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D342" s="5"/>
+      <c r="E342" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="343">
-      <c r="B343" s="1"/>
-      <c r="C343" s="5"/>
-      <c r="D343" s="5"/>
-      <c r="E343" s="10"/>
+      <c r="A343" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E343" s="1"/>
       <c r="F343" s="1"/>
     </row>
     <row r="344">
-      <c r="B344" s="1"/>
-      <c r="C344" s="1"/>
-      <c r="D344" s="1"/>
-      <c r="E344" s="1"/>
-      <c r="F344" s="1"/>
+      <c r="A344" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C344" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D344" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E344" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F344" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="345">
-      <c r="B345" s="1"/>
-      <c r="C345" s="1"/>
-      <c r="D345" s="5"/>
-      <c r="E345" s="10"/>
+      <c r="A345" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E345" s="1"/>
       <c r="F345" s="1"/>
     </row>
     <row r="346">
-      <c r="B346" s="1"/>
-      <c r="C346" s="1"/>
-      <c r="D346" s="1"/>
-      <c r="E346" s="1"/>
-      <c r="F346" s="1"/>
+      <c r="A346" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D346" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E346" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F346" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="347">
-      <c r="B347" s="1"/>
-      <c r="C347" s="1"/>
-      <c r="D347" s="5"/>
-      <c r="E347" s="10"/>
+      <c r="A347" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E347" s="1"/>
       <c r="F347" s="1"/>
     </row>
+    <row r="348">
+      <c r="A348" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D348" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E348" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="349">
-      <c r="B349" s="1"/>
-      <c r="C349" s="1"/>
-      <c r="D349" s="1"/>
+      <c r="A349" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E349" s="1"/>
       <c r="F349" s="1"/>
     </row>
     <row r="350">
-      <c r="B350" s="1"/>
-      <c r="C350" s="5"/>
-      <c r="D350" s="5"/>
-      <c r="E350" s="7"/>
-      <c r="F350" s="1"/>
+      <c r="A350" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C350" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D350" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E350" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="351">
-      <c r="B351" s="1"/>
-      <c r="C351" s="1"/>
-      <c r="D351" s="1"/>
+      <c r="A351" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E351" s="1"/>
       <c r="F351" s="1"/>
     </row>
     <row r="352">
-      <c r="B352" s="1"/>
-      <c r="C352" s="1"/>
-      <c r="D352" s="5"/>
-      <c r="E352" s="10"/>
-      <c r="F352" s="1"/>
+      <c r="A352" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D352" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E352" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="353">
-      <c r="B353" s="1"/>
-      <c r="C353" s="1"/>
-      <c r="D353" s="1"/>
+      <c r="A353" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E353" s="1"/>
       <c r="F353" s="1"/>
     </row>
     <row r="354">
-      <c r="B354" s="1"/>
-      <c r="C354" s="1"/>
-      <c r="D354" s="5"/>
-      <c r="E354" s="10"/>
-      <c r="F354" s="1"/>
+      <c r="A354" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D354" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E354" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F354" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="355">
-      <c r="B355" s="1"/>
-      <c r="C355" s="1"/>
-      <c r="D355" s="1"/>
+      <c r="A355" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E355" s="1"/>
       <c r="F355" s="1"/>
     </row>
     <row r="356">
-      <c r="B356" s="1"/>
-      <c r="C356" s="5"/>
-      <c r="D356" s="5"/>
-      <c r="E356" s="10"/>
-      <c r="F356" s="1"/>
+      <c r="A356" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C356" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D356" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E356" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F356" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="357">
-      <c r="B357" s="1"/>
-      <c r="C357" s="1"/>
-      <c r="D357" s="1"/>
+      <c r="A357" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E357" s="1"/>
       <c r="F357" s="1"/>
     </row>
     <row r="358">
-      <c r="B358" s="1"/>
-      <c r="C358" s="1"/>
-      <c r="D358" s="5"/>
-      <c r="E358" s="10"/>
-      <c r="F358" s="1"/>
+      <c r="A358" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D358" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E358" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F358" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="359">
-      <c r="B359" s="1"/>
-      <c r="C359" s="1"/>
-      <c r="D359" s="1"/>
+      <c r="A359" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E359" s="1"/>
       <c r="F359" s="1"/>
     </row>
     <row r="360">
-      <c r="B360" s="1"/>
-      <c r="C360" s="1"/>
-      <c r="D360" s="5"/>
-      <c r="E360" s="10"/>
-      <c r="F360" s="1"/>
+      <c r="A360" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D360" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E360" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E361" s="1"/>
+      <c r="F361" s="1"/>
     </row>
     <row r="362">
-      <c r="B362" s="1"/>
-      <c r="C362" s="1"/>
-      <c r="D362" s="1"/>
-      <c r="E362" s="1"/>
-      <c r="F362" s="1"/>
+      <c r="A362" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D362" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E362" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="363">
-      <c r="B363" s="1"/>
-      <c r="C363" s="5"/>
-      <c r="D363" s="5"/>
-      <c r="E363" s="7"/>
+      <c r="A363" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E363" s="1"/>
       <c r="F363" s="1"/>
     </row>
     <row r="364">
-      <c r="B364" s="1"/>
-      <c r="C364" s="1"/>
-      <c r="D364" s="1"/>
-      <c r="E364" s="1"/>
-      <c r="F364" s="1"/>
+      <c r="A364" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C364" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D364" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E364" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="365">
-      <c r="B365" s="1"/>
-      <c r="C365" s="1"/>
-      <c r="D365" s="5"/>
-      <c r="E365" s="10"/>
+      <c r="A365" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E365" s="1"/>
       <c r="F365" s="1"/>
     </row>
     <row r="366">
-      <c r="B366" s="1"/>
-      <c r="C366" s="1"/>
-      <c r="D366" s="1"/>
-      <c r="E366" s="1"/>
-      <c r="F366" s="1"/>
+      <c r="A366" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C366" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D366" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E366" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="367">
-      <c r="B367" s="1"/>
-      <c r="C367" s="1"/>
-      <c r="D367" s="5"/>
-      <c r="E367" s="10"/>
+      <c r="A367" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E367" s="1"/>
       <c r="F367" s="1"/>
     </row>
     <row r="368">
-      <c r="B368" s="1"/>
-      <c r="C368" s="1"/>
-      <c r="D368" s="1"/>
-      <c r="E368" s="1"/>
-      <c r="F368" s="1"/>
+      <c r="A368" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D368" s="5"/>
+      <c r="E368" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F368" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="369">
-      <c r="B369" s="1"/>
-      <c r="C369" s="5"/>
-      <c r="D369" s="5"/>
-      <c r="E369" s="10"/>
+      <c r="A369" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E369" s="1"/>
       <c r="F369" s="1"/>
     </row>
     <row r="370">
-      <c r="B370" s="1"/>
-      <c r="C370" s="1"/>
-      <c r="D370" s="1"/>
-      <c r="E370" s="1"/>
-      <c r="F370" s="1"/>
+      <c r="A370" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D370" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E370" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="371">
-      <c r="B371" s="1"/>
-      <c r="C371" s="1"/>
-      <c r="D371" s="5"/>
-      <c r="E371" s="10"/>
+      <c r="A371" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E371" s="1"/>
       <c r="F371" s="1"/>
     </row>
     <row r="372">
-      <c r="B372" s="1"/>
-      <c r="C372" s="1"/>
-      <c r="D372" s="1"/>
-      <c r="E372" s="1"/>
-      <c r="F372" s="1"/>
+      <c r="A372" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D372" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E372" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F372" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="373">
-      <c r="B373" s="1"/>
-      <c r="C373" s="1"/>
-      <c r="D373" s="5"/>
-      <c r="E373" s="10"/>
+      <c r="A373" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E373" s="1"/>
       <c r="F373" s="1"/>
     </row>
+    <row r="374">
+      <c r="A374" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C374" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D374" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E374" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="375">
-      <c r="B375" s="1"/>
-      <c r="C375" s="1"/>
-      <c r="D375" s="1"/>
+      <c r="A375" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E375" s="1"/>
       <c r="F375" s="1"/>
     </row>
     <row r="376">
-      <c r="B376" s="1"/>
-      <c r="C376" s="5"/>
-      <c r="D376" s="5"/>
-      <c r="E376" s="7"/>
-      <c r="F376" s="1"/>
+      <c r="A376" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D376" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E376" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F376" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="377">
-      <c r="B377" s="1"/>
-      <c r="C377" s="1"/>
-      <c r="D377" s="1"/>
+      <c r="A377" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E377" s="1"/>
       <c r="F377" s="1"/>
     </row>
     <row r="378">
-      <c r="B378" s="1"/>
-      <c r="C378" s="1"/>
-      <c r="D378" s="5"/>
-      <c r="E378" s="10"/>
-      <c r="F378" s="1"/>
+      <c r="A378" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D378" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E378" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="379">
-      <c r="B379" s="1"/>
-      <c r="C379" s="1"/>
-      <c r="D379" s="1"/>
+      <c r="A379" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E379" s="1"/>
       <c r="F379" s="1"/>
     </row>
     <row r="380">
-      <c r="B380" s="1"/>
-      <c r="C380" s="1"/>
-      <c r="D380" s="5"/>
-      <c r="E380" s="10"/>
-      <c r="F380" s="1"/>
+      <c r="A380" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D380" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E380" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="381">
-      <c r="B381" s="1"/>
-      <c r="C381" s="1"/>
-      <c r="D381" s="1"/>
+      <c r="A381" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D381" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E381" s="1"/>
       <c r="F381" s="1"/>
     </row>
     <row r="382">
-      <c r="B382" s="1"/>
-      <c r="C382" s="5"/>
-      <c r="D382" s="5"/>
-      <c r="E382" s="10"/>
-      <c r="F382" s="1"/>
+      <c r="A382" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D382" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E382" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F382" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="383">
-      <c r="B383" s="1"/>
-      <c r="C383" s="1"/>
-      <c r="D383" s="1"/>
+      <c r="A383" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E383" s="1"/>
       <c r="F383" s="1"/>
     </row>
     <row r="384">
-      <c r="B384" s="1"/>
-      <c r="C384" s="1"/>
+      <c r="A384" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C384" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D384" s="5"/>
-      <c r="E384" s="10"/>
-      <c r="F384" s="1"/>
+      <c r="E384" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F384" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="385">
-      <c r="B385" s="1"/>
-      <c r="C385" s="1"/>
-      <c r="D385" s="1"/>
+      <c r="A385" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E385" s="1"/>
       <c r="F385" s="1"/>
     </row>
     <row r="386">
-      <c r="B386" s="1"/>
-      <c r="C386" s="1"/>
-      <c r="D386" s="5"/>
-      <c r="E386" s="10"/>
-      <c r="F386" s="1"/>
+      <c r="A386" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D386" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E386" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F386" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D387" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E387" s="1"/>
+      <c r="F387" s="1"/>
     </row>
     <row r="388">
-      <c r="B388" s="1"/>
-      <c r="C388" s="1"/>
-      <c r="D388" s="1"/>
-      <c r="E388" s="1"/>
-      <c r="F388" s="1"/>
+      <c r="A388" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D388" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E388" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F388" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="389">
-      <c r="B389" s="1"/>
-      <c r="C389" s="5"/>
-      <c r="D389" s="5"/>
-      <c r="E389" s="7"/>
+      <c r="A389" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E389" s="1"/>
       <c r="F389" s="1"/>
     </row>
     <row r="390">
-      <c r="B390" s="1"/>
-      <c r="C390" s="1"/>
-      <c r="D390" s="1"/>
-      <c r="E390" s="1"/>
-      <c r="F390" s="1"/>
+      <c r="A390" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D390" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E390" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F390" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="391">
-      <c r="B391" s="1"/>
-      <c r="C391" s="1"/>
-      <c r="D391" s="5"/>
-      <c r="E391" s="10"/>
+      <c r="A391" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E391" s="1"/>
       <c r="F391" s="1"/>
     </row>
     <row r="392">
-      <c r="B392" s="1"/>
-      <c r="C392" s="1"/>
-      <c r="D392" s="1"/>
-      <c r="E392" s="1"/>
-      <c r="F392" s="1"/>
+      <c r="A392" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D392" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E392" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F392" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="393">
-      <c r="B393" s="1"/>
-      <c r="C393" s="1"/>
-      <c r="D393" s="5"/>
-      <c r="E393" s="10"/>
+      <c r="A393" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E393" s="1"/>
       <c r="F393" s="1"/>
     </row>
     <row r="394">
-      <c r="B394" s="1"/>
-      <c r="C394" s="1"/>
-      <c r="D394" s="1"/>
-      <c r="E394" s="1"/>
-      <c r="F394" s="1"/>
+      <c r="A394" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D394" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E394" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="395">
-      <c r="B395" s="1"/>
-      <c r="C395" s="5"/>
-      <c r="D395" s="5"/>
-      <c r="E395" s="10"/>
+      <c r="A395" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E395" s="1"/>
       <c r="F395" s="1"/>
     </row>
     <row r="396">
-      <c r="B396" s="1"/>
-      <c r="C396" s="1"/>
-      <c r="D396" s="1"/>
-      <c r="E396" s="1"/>
-      <c r="F396" s="1"/>
+      <c r="A396" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D396" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E396" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="397">
-      <c r="B397" s="1"/>
-      <c r="C397" s="1"/>
-      <c r="D397" s="5"/>
-      <c r="E397" s="10"/>
+      <c r="A397" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E397" s="1"/>
       <c r="F397" s="1"/>
     </row>
     <row r="398">
-      <c r="B398" s="1"/>
-      <c r="C398" s="1"/>
-      <c r="D398" s="1"/>
-      <c r="E398" s="1"/>
-      <c r="F398" s="1"/>
+      <c r="A398" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D398" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E398" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="399">
-      <c r="B399" s="1"/>
-      <c r="C399" s="1"/>
-      <c r="D399" s="5"/>
-      <c r="E399" s="10"/>
+      <c r="A399" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E399" s="1"/>
       <c r="F399" s="1"/>
     </row>
+    <row r="400">
+      <c r="A400" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C400" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D400" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E400" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="401">
-      <c r="B401" s="1"/>
-      <c r="C401" s="1"/>
-      <c r="D401" s="1"/>
+      <c r="A401" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D401" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E401" s="1"/>
       <c r="F401" s="1"/>
     </row>
     <row r="402">
-      <c r="B402" s="1"/>
-      <c r="C402" s="5"/>
-      <c r="D402" s="5"/>
-      <c r="E402" s="7"/>
-      <c r="F402" s="1"/>
+      <c r="A402" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D402" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E402" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="403">
-      <c r="B403" s="1"/>
-      <c r="C403" s="1"/>
-      <c r="D403" s="1"/>
+      <c r="A403" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D403" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E403" s="1"/>
       <c r="F403" s="1"/>
     </row>
     <row r="404">
-      <c r="B404" s="1"/>
-      <c r="C404" s="1"/>
-      <c r="D404" s="5"/>
-      <c r="E404" s="10"/>
-      <c r="F404" s="1"/>
+      <c r="A404" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C404" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D404" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E404" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="405">
-      <c r="B405" s="1"/>
-      <c r="C405" s="1"/>
-      <c r="D405" s="1"/>
+      <c r="A405" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E405" s="1"/>
       <c r="F405" s="1"/>
     </row>
     <row r="406">
-      <c r="B406" s="1"/>
-      <c r="C406" s="1"/>
+      <c r="A406" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D406" s="5"/>
-      <c r="E406" s="10"/>
-      <c r="F406" s="1"/>
+      <c r="E406" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F406" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="407">
-      <c r="B407" s="1"/>
-      <c r="C407" s="1"/>
-      <c r="D407" s="1"/>
+      <c r="A407" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E407" s="1"/>
       <c r="F407" s="1"/>
     </row>
     <row r="408">
-      <c r="B408" s="1"/>
-      <c r="C408" s="5"/>
-      <c r="D408" s="5"/>
-      <c r="E408" s="10"/>
-      <c r="F408" s="1"/>
+      <c r="A408" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D408" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E408" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F408" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="409">
-      <c r="B409" s="1"/>
-      <c r="C409" s="1"/>
-      <c r="D409" s="1"/>
+      <c r="A409" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E409" s="1"/>
       <c r="F409" s="1"/>
     </row>
     <row r="410">
-      <c r="B410" s="1"/>
-      <c r="C410" s="1"/>
-      <c r="D410" s="5"/>
-      <c r="E410" s="10"/>
-      <c r="F410" s="1"/>
+      <c r="A410" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C410" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D410" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E410" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F410" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="411">
-      <c r="B411" s="1"/>
-      <c r="C411" s="1"/>
-      <c r="D411" s="1"/>
+      <c r="A411" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E411" s="1"/>
       <c r="F411" s="1"/>
     </row>
     <row r="412">
-      <c r="B412" s="1"/>
-      <c r="C412" s="1"/>
-      <c r="D412" s="5"/>
-      <c r="E412" s="10"/>
-      <c r="F412" s="1"/>
+      <c r="A412" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D412" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E412" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F412" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E413" s="1"/>
+      <c r="F413" s="1"/>
     </row>
     <row r="414">
-      <c r="B414" s="1"/>
-      <c r="C414" s="1"/>
-      <c r="D414" s="1"/>
-      <c r="E414" s="1"/>
-      <c r="F414" s="1"/>
+      <c r="A414" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D414" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E414" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F414" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="415">
-      <c r="B415" s="1"/>
-      <c r="C415" s="5"/>
-      <c r="D415" s="5"/>
-      <c r="E415" s="7"/>
+      <c r="A415" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E415" s="1"/>
       <c r="F415" s="1"/>
     </row>
     <row r="416">
-      <c r="B416" s="1"/>
-      <c r="C416" s="1"/>
-      <c r="D416" s="1"/>
-      <c r="E416" s="1"/>
-      <c r="F416" s="1"/>
+      <c r="A416" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C416" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D416" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E416" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F416" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="417">
-      <c r="B417" s="1"/>
-      <c r="C417" s="1"/>
-      <c r="D417" s="5"/>
-      <c r="E417" s="10"/>
+      <c r="A417" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E417" s="1"/>
       <c r="F417" s="1"/>
     </row>
     <row r="418">
-      <c r="B418" s="1"/>
-      <c r="C418" s="1"/>
-      <c r="D418" s="1"/>
-      <c r="E418" s="1"/>
-      <c r="F418" s="1"/>
+      <c r="A418" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D418" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E418" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F418" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="419">
-      <c r="B419" s="1"/>
-      <c r="C419" s="1"/>
-      <c r="D419" s="5"/>
-      <c r="E419" s="10"/>
+      <c r="A419" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E419" s="1"/>
       <c r="F419" s="1"/>
     </row>
     <row r="420">
-      <c r="B420" s="1"/>
-      <c r="C420" s="1"/>
-      <c r="D420" s="1"/>
-      <c r="E420" s="1"/>
-      <c r="F420" s="1"/>
+      <c r="A420" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D420" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E420" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F420" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="421">
-      <c r="B421" s="1"/>
-      <c r="C421" s="5"/>
-      <c r="D421" s="5"/>
-      <c r="E421" s="10"/>
+      <c r="A421" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D421" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E421" s="1"/>
       <c r="F421" s="1"/>
     </row>
     <row r="422">
-      <c r="B422" s="1"/>
-      <c r="C422" s="1"/>
-      <c r="D422" s="1"/>
-      <c r="E422" s="1"/>
-      <c r="F422" s="1"/>
+      <c r="A422" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C422" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D422" s="5"/>
+      <c r="E422" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F422" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="423">
-      <c r="B423" s="1"/>
-      <c r="C423" s="1"/>
-      <c r="D423" s="5"/>
-      <c r="E423" s="10"/>
+      <c r="A423" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E423" s="1"/>
       <c r="F423" s="1"/>
     </row>
     <row r="424">
-      <c r="B424" s="1"/>
-      <c r="C424" s="1"/>
-      <c r="D424" s="1"/>
-      <c r="E424" s="1"/>
-      <c r="F424" s="1"/>
+      <c r="A424" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D424" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E424" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F424" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="425">
-      <c r="B425" s="1"/>
-      <c r="C425" s="1"/>
-      <c r="D425" s="5"/>
-      <c r="E425" s="10"/>
+      <c r="A425" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B425" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E425" s="1"/>
       <c r="F425" s="1"/>
     </row>
+    <row r="426">
+      <c r="A426" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D426" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E426" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F426" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="427">
-      <c r="B427" s="1"/>
-      <c r="C427" s="1"/>
-      <c r="D427" s="1"/>
+      <c r="A427" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E427" s="1"/>
       <c r="F427" s="1"/>
     </row>
     <row r="428">
-      <c r="B428" s="1"/>
-      <c r="C428" s="5"/>
-      <c r="D428" s="5"/>
-      <c r="E428" s="7"/>
-      <c r="F428" s="1"/>
+      <c r="A428" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D428" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E428" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F428" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="429">
-      <c r="B429" s="1"/>
-      <c r="C429" s="1"/>
-      <c r="D429" s="1"/>
+      <c r="A429" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E429" s="1"/>
       <c r="F429" s="1"/>
     </row>
     <row r="430">
-      <c r="B430" s="1"/>
-      <c r="C430" s="1"/>
-      <c r="D430" s="5"/>
-      <c r="E430" s="10"/>
-      <c r="F430" s="1"/>
+      <c r="A430" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B430" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C430" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D430" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E430" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F430" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="431">
-      <c r="B431" s="1"/>
-      <c r="C431" s="1"/>
-      <c r="D431" s="1"/>
+      <c r="A431" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E431" s="1"/>
       <c r="F431" s="1"/>
     </row>
     <row r="432">
-      <c r="B432" s="1"/>
-      <c r="C432" s="1"/>
+      <c r="A432" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D432" s="5"/>
-      <c r="E432" s="10"/>
-      <c r="F432" s="1"/>
+      <c r="E432" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F432" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="433">
-      <c r="B433" s="1"/>
-      <c r="C433" s="1"/>
-      <c r="D433" s="1"/>
+      <c r="A433" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E433" s="1"/>
       <c r="F433" s="1"/>
     </row>
     <row r="434">
-      <c r="B434" s="1"/>
-      <c r="C434" s="5"/>
-      <c r="D434" s="5"/>
-      <c r="E434" s="10"/>
-      <c r="F434" s="1"/>
+      <c r="A434" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B434" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D434" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E434" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F434" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="435">
-      <c r="B435" s="1"/>
-      <c r="C435" s="1"/>
-      <c r="D435" s="1"/>
+      <c r="A435" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E435" s="1"/>
       <c r="F435" s="1"/>
     </row>
     <row r="436">
-      <c r="B436" s="1"/>
-      <c r="C436" s="1"/>
+      <c r="A436" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D436" s="5"/>
-      <c r="E436" s="10"/>
-      <c r="F436" s="1"/>
+      <c r="E436" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F436" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="437">
-      <c r="B437" s="1"/>
-      <c r="C437" s="1"/>
-      <c r="D437" s="1"/>
+      <c r="A437" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E437" s="1"/>
       <c r="F437" s="1"/>
     </row>
     <row r="438">
-      <c r="B438" s="1"/>
-      <c r="C438" s="1"/>
-      <c r="D438" s="5"/>
-      <c r="E438" s="10"/>
-      <c r="F438" s="1"/>
+      <c r="A438" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C438" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D438" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E438" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F438" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E439" s="1"/>
+      <c r="F439" s="1"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D440" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E440" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D441" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E441" s="1"/>
+      <c r="F441" s="1"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D442" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E442" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F442" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="B443" s="1"/>
+      <c r="C443" s="1"/>
+      <c r="D443" s="1"/>
+      <c r="E443" s="1"/>
+      <c r="F443" s="1"/>
+    </row>
+    <row r="444">
+      <c r="B444" s="1"/>
+      <c r="C444" s="1"/>
+      <c r="D444" s="5"/>
+      <c r="F444" s="1"/>
+    </row>
+    <row r="445">
+      <c r="B445" s="1"/>
+      <c r="C445" s="1"/>
+      <c r="D445" s="1"/>
+      <c r="E445" s="1"/>
+      <c r="F445" s="1"/>
+    </row>
+    <row r="446">
+      <c r="B446" s="1"/>
+      <c r="C446" s="5"/>
+      <c r="D446" s="5"/>
+      <c r="F446" s="1"/>
+    </row>
+    <row r="447">
+      <c r="B447" s="1"/>
+      <c r="C447" s="1"/>
+      <c r="D447" s="1"/>
+      <c r="E447" s="1"/>
+      <c r="F447" s="1"/>
+    </row>
+    <row r="448">
+      <c r="B448" s="1"/>
+      <c r="C448" s="1"/>
+      <c r="D448" s="5"/>
+      <c r="F448" s="1"/>
+    </row>
+    <row r="449">
+      <c r="B449" s="1"/>
+      <c r="C449" s="1"/>
+      <c r="D449" s="1"/>
+      <c r="E449" s="1"/>
+      <c r="F449" s="1"/>
+    </row>
+    <row r="450">
+      <c r="B450" s="1"/>
+      <c r="C450" s="1"/>
+      <c r="D450" s="5"/>
+      <c r="F450" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>